<commit_message>
admin access with dataSourceResource
</commit_message>
<xml_diff>
--- a/build/web/doc/ebook feature list.xlsx
+++ b/build/web/doc/ebook feature list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leepeng/Documents/myWebProject/myprojects/bookstore/web/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{259EED0E-A7F9-3D43-AE51-B19D36F07DE2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DD6DEC6-18AF-104E-9A95-A2F954F2F162}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="18020" windowHeight="19380" xr2:uid="{D4DC86BC-6AE8-914B-A8E6-8059AD2AE09E}"/>
+    <workbookView xWindow="-20" yWindow="460" windowWidth="15820" windowHeight="21140" xr2:uid="{D4DC86BC-6AE8-914B-A8E6-8059AD2AE09E}"/>
   </bookViews>
   <sheets>
     <sheet name="feature" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="29">
   <si>
     <t>account</t>
   </si>
@@ -110,6 +110,9 @@
   </si>
   <si>
     <t>book</t>
+  </si>
+  <si>
+    <t>issue ,can not populate order data into db</t>
   </si>
 </sst>
 </file>
@@ -125,12 +128,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -145,8 +154,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -464,7 +474,7 @@
   <dimension ref="B1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -563,11 +573,17 @@
       <c r="D8" t="s">
         <v>22</v>
       </c>
+      <c r="E8" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C9" t="s">
         <v>24</v>
       </c>
+      <c r="E9" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
@@ -579,11 +595,17 @@
       <c r="D11" t="s">
         <v>2</v>
       </c>
+      <c r="E11" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C12" t="s">
         <v>5</v>
       </c>
+      <c r="E12" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
@@ -591,6 +613,9 @@
       </c>
       <c r="D13" t="s">
         <v>3</v>
+      </c>
+      <c r="E13" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
admin login, admin insert book
</commit_message>
<xml_diff>
--- a/build/web/doc/ebook feature list.xlsx
+++ b/build/web/doc/ebook feature list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leepeng/Documents/myWebProject/myprojects/bookstore/web/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DD6DEC6-18AF-104E-9A95-A2F954F2F162}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CF53887-47D0-774B-9840-3628895F17A7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="460" windowWidth="15820" windowHeight="21140" xr2:uid="{D4DC86BC-6AE8-914B-A8E6-8059AD2AE09E}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="15820" windowHeight="21140" xr2:uid="{D4DC86BC-6AE8-914B-A8E6-8059AD2AE09E}"/>
   </bookViews>
   <sheets>
     <sheet name="feature" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="45">
   <si>
     <t>account</t>
   </si>
@@ -76,9 +76,6 @@
     <t>ajax JS java</t>
   </si>
   <si>
-    <t>security</t>
-  </si>
-  <si>
     <t>update</t>
   </si>
   <si>
@@ -113,6 +110,57 @@
   </si>
   <si>
     <t>issue ,can not populate order data into db</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>May</t>
+  </si>
+  <si>
+    <t>insert book</t>
+  </si>
+  <si>
+    <t>update book</t>
+  </si>
+  <si>
+    <t>delete book</t>
+  </si>
+  <si>
+    <t>search book by criteira</t>
+  </si>
+  <si>
+    <t>authentication</t>
+  </si>
+  <si>
+    <t xml:space="preserve">load data </t>
+  </si>
+  <si>
+    <t>show data in the table</t>
+  </si>
+  <si>
+    <t>add photo</t>
+  </si>
+  <si>
+    <t>show data in multipages</t>
+  </si>
+  <si>
+    <t>open</t>
+  </si>
+  <si>
+    <t>search book title</t>
+  </si>
+  <si>
+    <t>logout</t>
+  </si>
+  <si>
+    <t>session invalidate</t>
+  </si>
+  <si>
+    <t>remark</t>
+  </si>
+  <si>
+    <t>sub-features</t>
   </si>
 </sst>
 </file>
@@ -128,7 +176,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -138,6 +186,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -154,9 +208,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -471,104 +527,127 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69A3EAB5-8184-574C-BDC6-076B1B07534B}">
-  <dimension ref="B1:F16"/>
+  <dimension ref="B1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4.83203125" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" customWidth="1"/>
+    <col min="3" max="3" width="25.5" customWidth="1"/>
+    <col min="7" max="7" width="21.33203125" customWidth="1"/>
+    <col min="8" max="8" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>11</v>
       </c>
+      <c r="C1" t="s">
+        <v>44</v>
+      </c>
       <c r="D1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E1" t="s">
         <v>12</v>
       </c>
       <c r="F1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="H1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="C5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
         <v>0</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C6" t="s">
         <v>7</v>
       </c>
-      <c r="D3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C4" t="s">
+      <c r="D6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C7" t="s">
         <v>8</v>
       </c>
-      <c r="D4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C7" t="s">
-        <v>18</v>
+      <c r="D7" t="s">
+        <v>22</v>
       </c>
       <c r="E7" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B8" t="s">
-        <v>19</v>
-      </c>
+      <c r="F7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C8" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="D8" t="s">
         <v>22</v>
@@ -576,69 +655,171 @@
       <c r="E8" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="H8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>1</v>
+      </c>
       <c r="C9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="F14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
         <v>24</v>
       </c>
-      <c r="E9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B11" t="s">
+      <c r="D15" t="s">
         <v>2</v>
       </c>
-      <c r="C11" t="s">
+      <c r="E15" t="s">
+        <v>13</v>
+      </c>
+      <c r="F15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C16" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" t="s">
+        <v>13</v>
+      </c>
+      <c r="F17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" t="s">
+        <v>4</v>
+      </c>
+      <c r="E18" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" s="2">
+        <v>43982</v>
+      </c>
+      <c r="G18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C19" t="s">
+        <v>30</v>
+      </c>
+      <c r="F19" s="2">
+        <v>43983</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C20" t="s">
+        <v>31</v>
+      </c>
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C21" t="s">
+        <v>32</v>
+      </c>
+      <c r="F21" s="2"/>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C22" t="s">
+        <v>33</v>
+      </c>
+      <c r="F22" s="2"/>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C23" t="s">
         <v>25</v>
       </c>
-      <c r="D11" t="s">
-        <v>2</v>
-      </c>
-      <c r="E11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C12" t="s">
-        <v>5</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B13" t="s">
-        <v>3</v>
-      </c>
-      <c r="D13" t="s">
-        <v>3</v>
-      </c>
-      <c r="E13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B14" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C15" t="s">
-        <v>26</v>
-      </c>
-      <c r="F15" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="C16" t="s">
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C24" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
pagination with block & list view
</commit_message>
<xml_diff>
--- a/build/web/doc/ebook feature list.xlsx
+++ b/build/web/doc/ebook feature list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leepeng/Documents/myWebProject/myprojects/bookstore/web/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CF53887-47D0-774B-9840-3628895F17A7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2515AC58-A333-144A-9F39-C07AE82A6A97}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="15820" windowHeight="21140" xr2:uid="{D4DC86BC-6AE8-914B-A8E6-8059AD2AE09E}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="16280" windowHeight="21140" xr2:uid="{D4DC86BC-6AE8-914B-A8E6-8059AD2AE09E}"/>
   </bookViews>
   <sheets>
     <sheet name="feature" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="51">
   <si>
     <t>account</t>
   </si>
@@ -161,6 +161,24 @@
   </si>
   <si>
     <t>sub-features</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>post</t>
+  </si>
+  <si>
+    <t>review</t>
+  </si>
+  <si>
+    <t>view search results by different criteria</t>
+  </si>
+  <si>
+    <t>/ebook/images/</t>
+  </si>
+  <si>
+    <t>view user</t>
   </si>
 </sst>
 </file>
@@ -176,7 +194,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -195,6 +213,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -208,11 +232,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="16" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -527,16 +553,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69A3EAB5-8184-574C-BDC6-076B1B07534B}">
-  <dimension ref="B1:H24"/>
+  <dimension ref="B1:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.83203125" customWidth="1"/>
-    <col min="3" max="3" width="25.5" customWidth="1"/>
+    <col min="1" max="1" width="3.1640625" customWidth="1"/>
+    <col min="3" max="3" width="26.33203125" customWidth="1"/>
+    <col min="4" max="4" width="10.5" customWidth="1"/>
+    <col min="5" max="5" width="8.6640625" customWidth="1"/>
     <col min="7" max="7" width="21.33203125" customWidth="1"/>
     <col min="8" max="8" width="17" customWidth="1"/>
   </cols>
@@ -582,16 +610,25 @@
       <c r="C3" t="s">
         <v>37</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>39</v>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="2">
+        <v>43983</v>
+      </c>
+      <c r="H3" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C4" t="s">
         <v>38</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>39</v>
+      <c r="E4" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" s="5">
+        <v>43984</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.2">
@@ -615,25 +652,19 @@
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B6" t="s">
+      <c r="C6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
         <v>0</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C7" t="s">
         <v>7</v>
-      </c>
-      <c r="D6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="C7" t="s">
-        <v>8</v>
       </c>
       <c r="D7" t="s">
         <v>22</v>
@@ -647,7 +678,7 @@
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C8" t="s">
-        <v>41</v>
+        <v>8</v>
       </c>
       <c r="D8" t="s">
         <v>22</v>
@@ -655,27 +686,30 @@
       <c r="E8" t="s">
         <v>13</v>
       </c>
-      <c r="H8" t="s">
+      <c r="F8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B9" t="s">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
         <v>1</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C10" t="s">
         <v>9</v>
-      </c>
-      <c r="E9" t="s">
-        <v>13</v>
-      </c>
-      <c r="F9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="C10" t="s">
-        <v>16</v>
       </c>
       <c r="E10" t="s">
         <v>13</v>
@@ -686,141 +720,219 @@
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C12" t="s">
         <v>17</v>
       </c>
-      <c r="E11" t="s">
-        <v>13</v>
-      </c>
-      <c r="F11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B12" t="s">
+      <c r="E12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
         <v>18</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" t="s">
         <v>19</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D13" t="s">
         <v>21</v>
       </c>
-      <c r="E12" t="s">
-        <v>13</v>
-      </c>
-      <c r="F12" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="C13" t="s">
+      <c r="E13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C14" t="s">
         <v>23</v>
       </c>
-      <c r="E13" t="s">
-        <v>13</v>
-      </c>
-      <c r="F13" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="E14" t="s">
+        <v>13</v>
+      </c>
       <c r="F14" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B15" t="s">
+      <c r="F15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
         <v>2</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C16" t="s">
         <v>24</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D16" t="s">
         <v>2</v>
-      </c>
-      <c r="E15" t="s">
-        <v>13</v>
-      </c>
-      <c r="F15" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="C16" t="s">
-        <v>5</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="F16" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B17" t="s">
-        <v>3</v>
-      </c>
-      <c r="D17" t="s">
-        <v>3</v>
-      </c>
-      <c r="E17" t="s">
-        <v>13</v>
-      </c>
-      <c r="F17" t="s">
-        <v>29</v>
-      </c>
+      <c r="C17" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" s="1"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E18" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
         <v>4</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C19" t="s">
         <v>7</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D19" t="s">
         <v>4</v>
       </c>
-      <c r="E18" t="s">
-        <v>13</v>
-      </c>
-      <c r="F18" s="2">
+      <c r="E19" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19" s="2">
         <v>43982</v>
       </c>
-      <c r="G18" t="s">
+      <c r="G19" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C19" t="s">
-        <v>30</v>
-      </c>
-      <c r="F19" s="2">
-        <v>43983</v>
-      </c>
-    </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C20" t="s">
-        <v>31</v>
-      </c>
       <c r="F20" s="2"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C21" t="s">
-        <v>32</v>
-      </c>
-      <c r="F21" s="2"/>
+        <v>30</v>
+      </c>
+      <c r="E21" t="s">
+        <v>13</v>
+      </c>
+      <c r="F21" s="2">
+        <v>43983</v>
+      </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C22" t="s">
-        <v>33</v>
-      </c>
-      <c r="F22" s="2"/>
+        <v>31</v>
+      </c>
+      <c r="E22" t="s">
+        <v>13</v>
+      </c>
+      <c r="F22" s="2">
+        <v>43983</v>
+      </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C23" t="s">
-        <v>25</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F23" s="2"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C24" t="s">
+        <v>50</v>
+      </c>
+      <c r="E24" s="3"/>
+      <c r="F24" s="2"/>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C25" t="s">
+        <v>33</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F25" s="2"/>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C26" t="s">
+        <v>25</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C27" t="s">
         <v>6</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E28" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>45</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E30" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
+        <v>46</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E32" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>47</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
grid and list view
</commit_message>
<xml_diff>
--- a/build/web/doc/ebook feature list.xlsx
+++ b/build/web/doc/ebook feature list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leepeng/Documents/myWebProject/myprojects/bookstore/web/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2515AC58-A333-144A-9F39-C07AE82A6A97}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB896819-7651-F74D-A90A-F12B93C84F88}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="16280" windowHeight="21140" xr2:uid="{D4DC86BC-6AE8-914B-A8E6-8059AD2AE09E}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="55">
   <si>
     <t>account</t>
   </si>
@@ -179,19 +179,37 @@
   </si>
   <si>
     <t>view user</t>
+  </si>
+  <si>
+    <t>import js</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CANNOT USE module in script. </t>
+  </si>
+  <si>
+    <t>cannot inser order to database order table</t>
+  </si>
+  <si>
+    <t>grid or list view</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -237,8 +255,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="16" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -553,10 +573,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69A3EAB5-8184-574C-BDC6-076B1B07534B}">
-  <dimension ref="B1:H33"/>
+  <dimension ref="B1:H37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -624,10 +644,10 @@
       <c r="C4" t="s">
         <v>38</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F4" s="5">
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="4">
         <v>43984</v>
       </c>
     </row>
@@ -660,25 +680,22 @@
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
+      <c r="C7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="2">
+        <v>43985</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
         <v>0</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C8" t="s">
         <v>7</v>
-      </c>
-      <c r="D7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="C8" t="s">
-        <v>8</v>
       </c>
       <c r="D8" t="s">
         <v>22</v>
@@ -692,7 +709,7 @@
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C9" t="s">
-        <v>41</v>
+        <v>8</v>
       </c>
       <c r="D9" t="s">
         <v>22</v>
@@ -700,27 +717,30 @@
       <c r="E9" t="s">
         <v>13</v>
       </c>
-      <c r="H9" t="s">
+      <c r="F9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H10" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B10" t="s">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
         <v>1</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" t="s">
         <v>9</v>
-      </c>
-      <c r="E10" t="s">
-        <v>13</v>
-      </c>
-      <c r="F10" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="C11" t="s">
-        <v>16</v>
       </c>
       <c r="E11" t="s">
         <v>13</v>
@@ -731,122 +751,122 @@
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C13" t="s">
         <v>17</v>
       </c>
-      <c r="E12" t="s">
-        <v>13</v>
-      </c>
-      <c r="F12" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B13" t="s">
+      <c r="E13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
         <v>18</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" t="s">
         <v>19</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D14" t="s">
         <v>21</v>
       </c>
-      <c r="E13" t="s">
-        <v>13</v>
-      </c>
-      <c r="F13" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="C14" t="s">
+      <c r="E14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C15" t="s">
         <v>23</v>
       </c>
-      <c r="E14" t="s">
-        <v>13</v>
-      </c>
-      <c r="F14" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="E15" t="s">
+        <v>13</v>
+      </c>
       <c r="F15" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B16" t="s">
+      <c r="F16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
         <v>2</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C17" t="s">
         <v>24</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D17" t="s">
         <v>2</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F16" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C17" t="s">
+      <c r="F17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C18" t="s">
         <v>5</v>
       </c>
-      <c r="E17" s="1"/>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B18" t="s">
-        <v>3</v>
-      </c>
-      <c r="D18" t="s">
-        <v>3</v>
-      </c>
-      <c r="E18" t="s">
-        <v>13</v>
-      </c>
-      <c r="F18" t="s">
-        <v>29</v>
-      </c>
+      <c r="E18" s="1"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
+        <v>3</v>
+      </c>
+      <c r="D19" t="s">
+        <v>3</v>
+      </c>
+      <c r="E19" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
         <v>4</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C20" t="s">
         <v>7</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D20" t="s">
         <v>4</v>
       </c>
-      <c r="E19" t="s">
-        <v>13</v>
-      </c>
-      <c r="F19" s="2">
+      <c r="E20" t="s">
+        <v>13</v>
+      </c>
+      <c r="F20" s="2">
         <v>43982</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G20" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="F20" s="2"/>
-    </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C21" t="s">
-        <v>30</v>
-      </c>
-      <c r="E21" t="s">
-        <v>13</v>
-      </c>
-      <c r="F21" s="2">
-        <v>43983</v>
-      </c>
+      <c r="F21" s="2"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E22" t="s">
         <v>13</v>
@@ -857,82 +877,101 @@
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C23" t="s">
-        <v>32</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="F23" s="2"/>
+        <v>31</v>
+      </c>
+      <c r="E23" t="s">
+        <v>13</v>
+      </c>
+      <c r="F23" s="2">
+        <v>43983</v>
+      </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C24" t="s">
-        <v>50</v>
-      </c>
-      <c r="E24" s="3"/>
+        <v>32</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="F24" s="2"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C25" t="s">
-        <v>33</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>39</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="E25" s="3"/>
       <c r="F25" s="2"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C26" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>39</v>
       </c>
+      <c r="F26" s="2"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C27" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C28" t="s">
+        <v>6</v>
+      </c>
       <c r="E28" s="3" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B29" t="s">
-        <v>45</v>
-      </c>
       <c r="E29" s="3" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>45</v>
+      </c>
       <c r="E30" s="3" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B31" t="s">
-        <v>46</v>
-      </c>
       <c r="E31" s="3" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>46</v>
+      </c>
       <c r="E32" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B33" t="s">
-        <v>47</v>
-      </c>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.2">
       <c r="E33" s="3" t="s">
         <v>39</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
+        <v>47</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C37" t="s">
+        <v>51</v>
+      </c>
+      <c r="F37" s="2">
+        <v>43985</v>
       </c>
     </row>
   </sheetData>
@@ -942,12 +981,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D355168-F2BD-C34D-982B-407DC10299F6}">
-  <dimension ref="A1"/>
+  <dimension ref="B2:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="2:2" ht="20" x14ac:dyDescent="0.2">
+      <c r="B2" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
admin update book part with sort by price
</commit_message>
<xml_diff>
--- a/build/web/doc/ebook feature list.xlsx
+++ b/build/web/doc/ebook feature list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leepeng/Documents/myWebProject/myprojects/bookstore/web/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB896819-7651-F74D-A90A-F12B93C84F88}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB38D267-DE60-3443-96AA-B5A250C0F3B4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="16280" windowHeight="21140" xr2:uid="{D4DC86BC-6AE8-914B-A8E6-8059AD2AE09E}"/>
   </bookViews>
@@ -233,7 +233,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -250,15 +250,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="16" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="16" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -576,7 +577,7 @@
   <dimension ref="B1:H37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -647,7 +648,7 @@
       <c r="E4" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="2">
         <v>43984</v>
       </c>
     </row>
@@ -675,8 +676,11 @@
       <c r="C6" t="s">
         <v>48</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="5" t="s">
         <v>39</v>
+      </c>
+      <c r="F6" s="6">
+        <v>43986</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.2">
@@ -990,7 +994,7 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="2" spans="2:2" ht="20" x14ac:dyDescent="0.2">
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>52</v>
       </c>
     </row>

</xml_diff>

<commit_message>
new pagination from DB directly
</commit_message>
<xml_diff>
--- a/build/web/doc/ebook feature list.xlsx
+++ b/build/web/doc/ebook feature list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leepeng/Documents/myWebProject/myprojects/bookstore/web/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB38D267-DE60-3443-96AA-B5A250C0F3B4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F90258B7-63D2-B045-A976-B6AE16BDF219}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="16280" windowHeight="21140" xr2:uid="{D4DC86BC-6AE8-914B-A8E6-8059AD2AE09E}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="59">
   <si>
     <t>account</t>
   </si>
@@ -191,6 +191,18 @@
   </si>
   <si>
     <t>grid or list view</t>
+  </si>
+  <si>
+    <t>collections.sort or JDBC order by</t>
+  </si>
+  <si>
+    <t>issue</t>
+  </si>
+  <si>
+    <t>cannot do it , error</t>
+  </si>
+  <si>
+    <t>suspend</t>
   </si>
 </sst>
 </file>
@@ -212,7 +224,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -231,12 +243,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -250,7 +256,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -258,8 +264,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="16" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -574,10 +578,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69A3EAB5-8184-574C-BDC6-076B1B07534B}">
-  <dimension ref="B1:H37"/>
+  <dimension ref="B1:I37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -590,7 +594,7 @@
     <col min="8" max="8" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>11</v>
       </c>
@@ -612,8 +616,11 @@
       <c r="H1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="I1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>35</v>
       </c>
@@ -627,7 +634,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C3" t="s">
         <v>37</v>
       </c>
@@ -641,7 +648,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C4" t="s">
         <v>38</v>
       </c>
@@ -652,7 +659,7 @@
         <v>43984</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>10</v>
       </c>
@@ -672,18 +679,21 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C6" t="s">
         <v>48</v>
       </c>
-      <c r="E6" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F6" s="6">
+      <c r="E6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="2">
         <v>43986</v>
       </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="G6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C7" t="s">
         <v>54</v>
       </c>
@@ -694,7 +704,7 @@
         <v>43985</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>0</v>
       </c>
@@ -711,7 +721,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C9" t="s">
         <v>8</v>
       </c>
@@ -725,7 +735,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C10" t="s">
         <v>41</v>
       </c>
@@ -739,7 +749,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>1</v>
       </c>
@@ -753,7 +763,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C12" t="s">
         <v>16</v>
       </c>
@@ -764,7 +774,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C13" t="s">
         <v>17</v>
       </c>
@@ -775,7 +785,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>18</v>
       </c>
@@ -792,7 +802,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C15" t="s">
         <v>23</v>
       </c>
@@ -803,12 +813,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.2">
       <c r="F16" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>2</v>
       </c>
@@ -819,19 +829,22 @@
         <v>2</v>
       </c>
       <c r="E17" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F17" t="s">
+        <v>29</v>
+      </c>
+      <c r="I17" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F17" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C18" t="s">
         <v>5</v>
       </c>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>3</v>
       </c>
@@ -845,7 +858,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>4</v>
       </c>
@@ -865,10 +878,10 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C22" t="s">
         <v>30</v>
       </c>
@@ -879,7 +892,7 @@
         <v>43983</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C23" t="s">
         <v>31</v>
       </c>
@@ -890,7 +903,7 @@
         <v>43983</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C24" t="s">
         <v>32</v>
       </c>
@@ -899,23 +912,28 @@
       </c>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C25" t="s">
         <v>50</v>
       </c>
       <c r="E25" s="3"/>
       <c r="F25" s="2"/>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C26" t="s">
         <v>33</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="F26" s="2"/>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+      <c r="F26" s="2">
+        <v>43986</v>
+      </c>
+      <c r="G26" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C27" t="s">
         <v>25</v>
       </c>
@@ -923,7 +941,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C28" t="s">
         <v>6</v>
       </c>
@@ -931,12 +949,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.2">
       <c r="E29" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>45</v>
       </c>
@@ -944,12 +962,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.2">
       <c r="E31" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>46</v>
       </c>
@@ -957,12 +975,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.2">
       <c r="E33" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
         <v>47</v>
       </c>
@@ -970,12 +988,18 @@
         <v>39</v>
       </c>
     </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C37" t="s">
         <v>51</v>
       </c>
+      <c r="E37" s="1" t="s">
+        <v>58</v>
+      </c>
       <c r="F37" s="2">
         <v>43985</v>
+      </c>
+      <c r="I37" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cart badge with quantity
</commit_message>
<xml_diff>
--- a/build/web/doc/ebook feature list.xlsx
+++ b/build/web/doc/ebook feature list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leepeng/Documents/myWebProject/myprojects/bookstore/web/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F90258B7-63D2-B045-A976-B6AE16BDF219}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53E8847E-8F8D-AD4C-8A8C-2CAA012F49B6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="16280" windowHeight="21140" xr2:uid="{D4DC86BC-6AE8-914B-A8E6-8059AD2AE09E}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="66">
   <si>
     <t>account</t>
   </si>
@@ -203,6 +203,27 @@
   </si>
   <si>
     <t>suspend</t>
+  </si>
+  <si>
+    <t>pagination</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ajax </t>
+  </si>
+  <si>
+    <t>cart items in sidebarB</t>
+  </si>
+  <si>
+    <t>browse</t>
+  </si>
+  <si>
+    <t>grid view/list view</t>
+  </si>
+  <si>
+    <t>cart totalprice in sidebarB</t>
+  </si>
+  <si>
+    <t>cart badge with quantity</t>
   </si>
 </sst>
 </file>
@@ -578,10 +599,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69A3EAB5-8184-574C-BDC6-076B1B07534B}">
-  <dimension ref="B1:I37"/>
+  <dimension ref="B1:I44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E20" sqref="E20:F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -684,14 +705,9 @@
         <v>48</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" s="2">
-        <v>43986</v>
-      </c>
-      <c r="G6" t="s">
-        <v>55</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="F6" s="2"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C7" t="s">
@@ -705,56 +721,36 @@
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B8" t="s">
-        <v>0</v>
-      </c>
       <c r="C8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" t="s">
-        <v>29</v>
+        <v>59</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="2">
+        <v>43988</v>
+      </c>
+      <c r="G8" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" t="s">
-        <v>13</v>
-      </c>
-      <c r="F9" t="s">
-        <v>29</v>
-      </c>
+      <c r="E9" s="3"/>
+      <c r="F9" s="2"/>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C10" t="s">
-        <v>41</v>
-      </c>
-      <c r="D10" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10" t="s">
-        <v>13</v>
-      </c>
-      <c r="H10" t="s">
-        <v>42</v>
-      </c>
+      <c r="E10" s="3"/>
+      <c r="F10" s="2"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C11" t="s">
-        <v>9</v>
+        <v>7</v>
+      </c>
+      <c r="D11" t="s">
+        <v>22</v>
       </c>
       <c r="E11" t="s">
         <v>13</v>
@@ -765,7 +761,10 @@
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C12" t="s">
-        <v>16</v>
+        <v>8</v>
+      </c>
+      <c r="D12" t="s">
+        <v>22</v>
       </c>
       <c r="E12" t="s">
         <v>13</v>
@@ -776,234 +775,315 @@
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C13" t="s">
-        <v>17</v>
+        <v>41</v>
+      </c>
+      <c r="D13" t="s">
+        <v>22</v>
       </c>
       <c r="E13" t="s">
         <v>13</v>
       </c>
-      <c r="F13" t="s">
-        <v>29</v>
+      <c r="H13" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="C14" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" t="s">
-        <v>21</v>
-      </c>
-      <c r="E14" t="s">
-        <v>13</v>
-      </c>
-      <c r="F14" t="s">
-        <v>29</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C15" t="s">
-        <v>23</v>
+        <v>61</v>
       </c>
       <c r="E15" t="s">
         <v>13</v>
       </c>
-      <c r="F15" t="s">
-        <v>29</v>
+      <c r="F15" s="2">
+        <v>43989</v>
       </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" t="s">
+        <v>13</v>
+      </c>
       <c r="F16" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B17" t="s">
-        <v>2</v>
-      </c>
       <c r="C17" t="s">
-        <v>24</v>
-      </c>
-      <c r="D17" t="s">
-        <v>2</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>58</v>
+        <v>16</v>
+      </c>
+      <c r="E17" t="s">
+        <v>13</v>
       </c>
       <c r="F17" t="s">
         <v>29</v>
       </c>
-      <c r="I17" s="1" t="s">
-        <v>27</v>
-      </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C18" t="s">
-        <v>5</v>
-      </c>
-      <c r="E18" s="1"/>
+        <v>17</v>
+      </c>
+      <c r="E18" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B19" t="s">
-        <v>3</v>
-      </c>
-      <c r="D19" t="s">
-        <v>3</v>
+      <c r="C19" t="s">
+        <v>64</v>
       </c>
       <c r="E19" t="s">
         <v>13</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19" s="2">
+        <v>43989</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C20" t="s">
+        <v>65</v>
+      </c>
+      <c r="E20" t="s">
+        <v>13</v>
+      </c>
+      <c r="F20" s="2">
+        <v>43989</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" t="s">
+        <v>21</v>
+      </c>
+      <c r="E21" t="s">
+        <v>13</v>
+      </c>
+      <c r="F21" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B20" t="s">
-        <v>4</v>
-      </c>
-      <c r="C20" t="s">
-        <v>7</v>
-      </c>
-      <c r="D20" t="s">
-        <v>4</v>
-      </c>
-      <c r="E20" t="s">
-        <v>13</v>
-      </c>
-      <c r="F20" s="2">
-        <v>43982</v>
-      </c>
-      <c r="G20" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="F21" s="2"/>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C22" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="E22" t="s">
         <v>13</v>
       </c>
-      <c r="F22" s="2">
-        <v>43983</v>
+      <c r="F22" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C23" t="s">
-        <v>31</v>
-      </c>
-      <c r="E23" t="s">
-        <v>13</v>
-      </c>
-      <c r="F23" s="2">
-        <v>43983</v>
+      <c r="F23" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>2</v>
+      </c>
       <c r="C24" t="s">
-        <v>32</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="F24" s="2"/>
+        <v>24</v>
+      </c>
+      <c r="D24" t="s">
+        <v>2</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F24" t="s">
+        <v>29</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C25" t="s">
-        <v>50</v>
-      </c>
-      <c r="E25" s="3"/>
-      <c r="F25" s="2"/>
+        <v>5</v>
+      </c>
+      <c r="E25" s="1"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C26" t="s">
-        <v>33</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F26" s="2">
-        <v>43986</v>
-      </c>
-      <c r="G26" t="s">
-        <v>55</v>
+      <c r="B26" t="s">
+        <v>3</v>
+      </c>
+      <c r="D26" t="s">
+        <v>3</v>
+      </c>
+      <c r="E26" t="s">
+        <v>13</v>
+      </c>
+      <c r="F26" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
+        <v>4</v>
+      </c>
       <c r="C27" t="s">
-        <v>25</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>39</v>
+        <v>7</v>
+      </c>
+      <c r="D27" t="s">
+        <v>4</v>
+      </c>
+      <c r="E27" t="s">
+        <v>13</v>
+      </c>
+      <c r="F27" s="2">
+        <v>43982</v>
+      </c>
+      <c r="G27" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C28" t="s">
-        <v>6</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>39</v>
-      </c>
+      <c r="F28" s="2"/>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="E29" s="3" t="s">
-        <v>39</v>
+      <c r="C29" t="s">
+        <v>30</v>
+      </c>
+      <c r="E29" t="s">
+        <v>13</v>
+      </c>
+      <c r="F29" s="2">
+        <v>43983</v>
       </c>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B30" t="s">
-        <v>45</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>39</v>
+      <c r="C30" t="s">
+        <v>31</v>
+      </c>
+      <c r="E30" t="s">
+        <v>13</v>
+      </c>
+      <c r="F30" s="2">
+        <v>43983</v>
       </c>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C31" t="s">
+        <v>32</v>
+      </c>
       <c r="E31" s="3" t="s">
         <v>39</v>
       </c>
+      <c r="F31" s="2"/>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B32" t="s">
-        <v>46</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>39</v>
-      </c>
+      <c r="C32" t="s">
+        <v>50</v>
+      </c>
+      <c r="E32" s="3"/>
+      <c r="F32" s="2"/>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C33" t="s">
+        <v>33</v>
+      </c>
       <c r="E33" s="3" t="s">
-        <v>39</v>
+        <v>13</v>
+      </c>
+      <c r="F33" s="2">
+        <v>43986</v>
+      </c>
+      <c r="G33" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B34" t="s">
-        <v>47</v>
+      <c r="C34" t="s">
+        <v>25</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>39</v>
       </c>
     </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C35" t="s">
+        <v>6</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="E36" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C37" t="s">
+      <c r="B37" t="s">
+        <v>45</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="E38" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B39" t="s">
+        <v>46</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="E40" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B41" t="s">
+        <v>47</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C44" t="s">
         <v>51</v>
       </c>
-      <c r="E37" s="1" t="s">
+      <c r="E44" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="F37" s="2">
+      <c r="F44" s="2">
         <v>43985</v>
       </c>
-      <c r="I37" t="s">
+      <c r="I44" t="s">
         <v>57</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 

</xml_diff>